<commit_message>
I-O Distribution Key.xlsx PL
</commit_message>
<xml_diff>
--- a/DimoPdfToExcelSln/DimoPdfToExcelWeb/wwwroot/Files/I-O Distribution Key.xlsx
+++ b/DimoPdfToExcelSln/DimoPdfToExcelWeb/wwwroot/Files/I-O Distribution Key.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hungarian BS" sheetId="1" r:id="rId1"/>
@@ -1087,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
@@ -2219,15 +2219,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2248,6 +2248,9 @@
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2256,6 +2259,9 @@
       <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -2270,6 +2276,9 @@
       <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2278,6 +2287,9 @@
       <c r="B7" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -2292,6 +2304,9 @@
       <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="C9">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -2306,6 +2321,9 @@
       <c r="B11" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -2314,6 +2332,9 @@
       <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
+      <c r="C12">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -2322,6 +2343,9 @@
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C13">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -2330,6 +2354,9 @@
       <c r="B14" s="11" t="s">
         <v>18</v>
       </c>
+      <c r="C14">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -2338,6 +2365,9 @@
       <c r="B15" s="10" t="s">
         <v>17</v>
       </c>
+      <c r="C15">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -2345,240 +2375,306 @@
       </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>186</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>187</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>188</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>190</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>192</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>194</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>195</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>196</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>197</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>198</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>200</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>199</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>202</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>203</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>204</v>
       </c>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>205</v>
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>201</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>208</v>
       </c>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>206</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>209</v>
       </c>
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>215</v>
       </c>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>216</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>2</v>
+      </c>
+      <c r="C48">
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>